<commit_message>
Shortened data for demo; retained original data in _long
</commit_message>
<xml_diff>
--- a/Tom/AOBrowseStore.xlsx
+++ b/Tom/AOBrowseStore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Selenium\Tom\AdvantageOnline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ScrumbagsRepos\AO-Responsiveness-Testing\Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8253D665-63B4-4F56-AB47-C132A05FDFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26359B1-AEDC-444A-8D07-09F6CF54BC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{28A10325-4D42-4F5D-BBD3-20C1305A8DDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{28A10325-4D42-4F5D-BBD3-20C1305A8DDE}"/>
   </bookViews>
   <sheets>
     <sheet name="TH_TC001" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="59">
   <si>
     <t>DT_compat</t>
   </si>
@@ -87,33 +87,15 @@
     <t>HP</t>
   </si>
   <si>
-    <t>Logitech</t>
-  </si>
-  <si>
-    <t>0.55 lb</t>
-  </si>
-  <si>
     <t>RED</t>
   </si>
   <si>
-    <t>1.0 lb</t>
-  </si>
-  <si>
-    <t>1.1 lb</t>
-  </si>
-  <si>
     <t>1.26 lb</t>
   </si>
   <si>
-    <t>1.95 lb</t>
-  </si>
-  <si>
     <t>BLUE</t>
   </si>
   <si>
-    <t>WHITE</t>
-  </si>
-  <si>
     <t>GRAY</t>
   </si>
   <si>
@@ -132,27 +114,15 @@
     <t>4</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>2.3 lb</t>
   </si>
   <si>
@@ -165,42 +135,15 @@
     <t>Windows 10</t>
   </si>
   <si>
-    <t>Windows 7 Professional 64</t>
-  </si>
-  <si>
     <t>Windows 8.1</t>
   </si>
   <si>
     <t>3.2 lb</t>
   </si>
   <si>
-    <t>7.25 lb</t>
-  </si>
-  <si>
-    <t>4.96 lb</t>
-  </si>
-  <si>
-    <t>4 lb</t>
-  </si>
-  <si>
-    <t>3.21 lb</t>
-  </si>
-  <si>
-    <t>7.42 lb</t>
-  </si>
-  <si>
     <t>PURPLE</t>
   </si>
   <si>
-    <t xml:space="preserve">3.17 lb </t>
-  </si>
-  <si>
-    <t>5.51 lb</t>
-  </si>
-  <si>
-    <t>3.4 lb</t>
-  </si>
-  <si>
     <t>DT_scroller</t>
   </si>
   <si>
@@ -219,9 +162,6 @@
     <t>0.03 lb</t>
   </si>
   <si>
-    <t>0.07 lb</t>
-  </si>
-  <si>
     <t xml:space="preserve">BLACK </t>
   </si>
   <si>
@@ -237,88 +177,28 @@
     <t>129.00</t>
   </si>
   <si>
-    <t>44.99</t>
-  </si>
-  <si>
-    <t>169.99</t>
-  </si>
-  <si>
-    <t>84.99</t>
-  </si>
-  <si>
-    <t>200.00</t>
-  </si>
-  <si>
-    <t>49.99</t>
-  </si>
-  <si>
     <t>299.99</t>
   </si>
   <si>
     <t>1261.99</t>
   </si>
   <si>
-    <t>849.99</t>
-  </si>
-  <si>
-    <t>699.99</t>
-  </si>
-  <si>
-    <t>519.99</t>
-  </si>
-  <si>
-    <t>449.99</t>
-  </si>
-  <si>
-    <t>549.99</t>
-  </si>
-  <si>
-    <t>319.99</t>
-  </si>
-  <si>
-    <t>1399.99</t>
-  </si>
-  <si>
     <t>179.99</t>
   </si>
   <si>
-    <t>1799.00</t>
-  </si>
-  <si>
     <t>1009.00</t>
   </si>
   <si>
     <t>1279.00</t>
   </si>
   <si>
-    <t>479.00</t>
-  </si>
-  <si>
     <t>59.99</t>
   </si>
   <si>
     <t>39.99</t>
   </si>
   <si>
-    <t>29.99</t>
-  </si>
-  <si>
-    <t>9.99</t>
-  </si>
-  <si>
-    <t>15.99</t>
-  </si>
-  <si>
-    <t>79.99</t>
-  </si>
-  <si>
     <t>279.95</t>
-  </si>
-  <si>
-    <t>13.99</t>
-  </si>
-  <si>
-    <t>50.99</t>
   </si>
   <si>
     <t>3.17 lb</t>
@@ -713,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C360406D-A0EC-4FCD-A6FC-571A77DF3CE8}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +613,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -751,13 +631,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -780,7 +660,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -798,121 +678,6 @@
         <v>11</v>
       </c>
       <c r="G3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="4">
         <v>1</v>
       </c>
     </row>
@@ -945,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -954,7 +719,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -965,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -976,16 +741,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -1000,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F68FE8-A49A-4CF3-AD70-E75FA9FEFE8B}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
@@ -1012,15 +777,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -1028,34 +793,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1069,7 +834,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G12" sqref="A4:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,16 +851,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1104,28 +869,28 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
@@ -1134,22 +899,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -1157,219 +922,30 @@
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
       <c r="H4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
       <c r="H5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
       <c r="H6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
       <c r="H7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
       <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
       <c r="H9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
       <c r="H10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
       <c r="H11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
       <c r="H12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1386,10 +962,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C11A34-4F49-422B-A43F-CF3963C42774}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E3"/>
+      <selection activeCell="E4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,24 +978,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1436,7 +1012,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1445,26 +1021,9 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1476,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5528C7F5-278A-4CF2-BD72-B5473E6328F9}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,27 +1051,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -1520,114 +1079,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1638,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71DF04E-6062-47E3-A32C-8CE600EEA918}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+      <selection activeCell="F5" sqref="A4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,13 +1117,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1671,12 +1132,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1685,7 +1146,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -1696,7 +1157,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1705,52 +1166,12 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="F3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1795,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1826,13 +1247,13 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -1864,13 +1285,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1879,24 +1300,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -1907,16 +1328,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -1946,16 +1367,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,10 +1398,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2009,13 +1430,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2023,7 +1444,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2034,7 +1455,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>

</xml_diff>